<commit_message>
Update automàtic: dades i banners [2026-02-20 09:35]
</commit_message>
<xml_diff>
--- a/src/data/resum_periode_meteocat.xlsx
+++ b/src/data/resum_periode_meteocat.xlsx
@@ -687,17 +687,17 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2026-02-20 09:15:32</t>
+          <t>2026-02-20 09:35:43</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>08:30</t>
+          <t>09:00</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>https://www.meteo.cat/observacions/xema/dades?codi=XJ&amp;dia=2026-02-20T08:30Z</t>
+          <t>https://www.meteo.cat/observacions/xema/dades?codi=XJ&amp;dia=2026-02-20T09:00Z</t>
         </is>
       </c>
       <c r="K2" t="n">
@@ -912,7 +912,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2026-02-20 09:15:34</t>
+          <t>2026-02-20 09:35:45</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2026-02-20 09:15:34</t>
+          <t>2026-02-20 09:35:45</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2026-02-20 09:15:34</t>
+          <t>2026-02-20 09:35:45</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -1587,7 +1587,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2026-02-20 09:15:34</t>
+          <t>2026-02-20 09:35:45</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -1851,7 +1851,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.meteo.cat/observacions/xema/dades?codi=XJ&amp;dia=2026-02-20T08:30Z</t>
+          <t>https://www.meteo.cat/observacions/xema/dades?codi=XJ&amp;dia=2026-02-20T09:00Z</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update automàtic: dades i banners [2026-02-20 09:49]
</commit_message>
<xml_diff>
--- a/src/data/resum_periode_meteocat.xlsx
+++ b/src/data/resum_periode_meteocat.xlsx
@@ -687,7 +687,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2026-02-20 09:45:28</t>
+          <t>2026-02-20 09:49:16</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -912,7 +912,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2026-02-20 09:45:30</t>
+          <t>2026-02-20 09:49:18</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2026-02-20 09:45:30</t>
+          <t>2026-02-20 09:49:18</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2026-02-20 09:45:30</t>
+          <t>2026-02-20 09:49:18</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -1587,7 +1587,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2026-02-20 09:45:30</t>
+          <t>2026-02-20 09:49:18</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">

</xml_diff>

<commit_message>
Update automàtic: dades i banners [2026-02-20 09:56]
</commit_message>
<xml_diff>
--- a/src/data/resum_periode_meteocat.xlsx
+++ b/src/data/resum_periode_meteocat.xlsx
@@ -687,7 +687,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2026-02-20 09:49:16</t>
+          <t>2026-02-20 09:56:47</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -912,7 +912,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2026-02-20 09:49:18</t>
+          <t>2026-02-20 09:56:49</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2026-02-20 09:49:18</t>
+          <t>2026-02-20 09:56:49</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2026-02-20 09:49:18</t>
+          <t>2026-02-20 09:56:49</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -1587,7 +1587,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2026-02-20 09:49:18</t>
+          <t>2026-02-20 09:56:49</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">

</xml_diff>

<commit_message>
Update automàtic: dades i banners [2026-02-20 10:15]
</commit_message>
<xml_diff>
--- a/src/data/resum_periode_meteocat.xlsx
+++ b/src/data/resum_periode_meteocat.xlsx
@@ -687,7 +687,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2026-02-20 10:10:55</t>
+          <t>2026-02-20 10:15:29</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -912,7 +912,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2026-02-20 10:10:57</t>
+          <t>2026-02-20 10:15:30</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2026-02-20 10:10:57</t>
+          <t>2026-02-20 10:15:30</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2026-02-20 10:10:57</t>
+          <t>2026-02-20 10:15:30</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -1587,7 +1587,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2026-02-20 10:10:57</t>
+          <t>2026-02-20 10:15:30</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">

</xml_diff>

<commit_message>
Update automàtic: dades i banners [2026-02-20 11:38]
</commit_message>
<xml_diff>
--- a/src/data/resum_periode_meteocat.xlsx
+++ b/src/data/resum_periode_meteocat.xlsx
@@ -687,17 +687,17 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2026-02-20 11:15:27</t>
+          <t>2026-02-20 11:38:39</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>10:30</t>
+          <t>11:00</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>https://www.meteo.cat/observacions/xema/dades?codi=XJ&amp;dia=2026-02-20T10:30Z</t>
+          <t>https://www.meteo.cat/observacions/xema/dades?codi=XJ&amp;dia=2026-02-20T11:00Z</t>
         </is>
       </c>
       <c r="K2" t="n">
@@ -912,7 +912,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2026-02-20 11:15:28</t>
+          <t>2026-02-20 11:38:41</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2026-02-20 11:15:28</t>
+          <t>2026-02-20 11:38:41</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2026-02-20 11:15:28</t>
+          <t>2026-02-20 11:38:41</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -1587,7 +1587,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2026-02-20 11:15:28</t>
+          <t>2026-02-20 11:38:41</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -1851,7 +1851,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.meteo.cat/observacions/xema/dades?codi=XJ&amp;dia=2026-02-20T10:30Z</t>
+          <t>https://www.meteo.cat/observacions/xema/dades?codi=XJ&amp;dia=2026-02-20T11:00Z</t>
         </is>
       </c>
     </row>

</xml_diff>